<commit_message>
Altium and Jupyter content update
</commit_message>
<xml_diff>
--- a/Électronique/Electronic budget planing.xlsx
+++ b/Électronique/Electronic budget planing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/matot9_ulaval_ca/Documents/Github/design3/Électronique/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="8_{F4AF0EF8-8E10-4CF9-8076-0BC56F572DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3360EB4-8A64-44DA-9C28-1AE34EEC9221}"/>
+  <xr:revisionPtr revIDLastSave="391" documentId="8_{F4AF0EF8-8E10-4CF9-8076-0BC56F572DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C3049B9-FB53-4485-87E1-116FBF965942}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{EB5A697F-0613-4937-9779-A2AEDA335630}"/>
   </bookViews>
@@ -253,8 +253,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ [$$-C0C]_ ;_ * \(#,##0.00\)\ [$$-C0C]_ ;_ * &quot;-&quot;??_)\ [$$-C0C]_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="0.000&quot; mA&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.0&quot; mA&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.000&quot; mA&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0&quot; mA&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -540,7 +540,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -644,44 +644,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -708,10 +689,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -719,6 +697,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1044,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14AF596-72B6-4068-B240-BE4D8ECB5EC6}">
   <dimension ref="B1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:J33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1069,23 +1056,23 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="2" spans="2:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="38"/>
-      <c r="M2" s="37" t="s">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
+      <c r="M2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="53"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="22" t="s">
@@ -1115,16 +1102,16 @@
       <c r="J3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="55" t="s">
+      <c r="M3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="56" t="s">
+      <c r="N3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="54" t="s">
+      <c r="P3" s="47" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1160,14 +1147,14 @@
       <c r="M4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="57">
+      <c r="N4" s="50">
         <f>SUM(J4:J5)</f>
         <v>4.28</v>
       </c>
-      <c r="O4" s="59">
+      <c r="O4" s="52">
         <v>10</v>
       </c>
-      <c r="P4" s="61">
+      <c r="P4" s="53">
         <f>O4*N4</f>
         <v>42.800000000000004</v>
       </c>
@@ -1204,16 +1191,16 @@
       <c r="M5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="52">
+      <c r="N5" s="45">
         <f>SUM(J4:J6)</f>
         <v>6.9600000000000009</v>
       </c>
-      <c r="O5" s="60">
-        <v>10</v>
-      </c>
-      <c r="P5" s="62">
+      <c r="O5" s="13">
+        <v>8</v>
+      </c>
+      <c r="P5" s="54">
         <f>O5*N5</f>
-        <v>69.600000000000009</v>
+        <v>55.680000000000007</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1269,18 +1256,18 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="38"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="23"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -1440,17 +1427,17 @@
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="2:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="38"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="57"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
@@ -1547,17 +1534,17 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="38"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="57"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1664,17 +1651,17 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="38"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="57"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="22" t="s">
@@ -1709,22 +1696,22 @@
       <c r="B30" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="2">
         <v>1</v>
       </c>
       <c r="I30" s="6">
@@ -1739,22 +1726,22 @@
       <c r="B31" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="2">
         <v>1</v>
       </c>
       <c r="I31" s="6">
@@ -1769,22 +1756,22 @@
       <c r="B32" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="2">
         <v>1</v>
       </c>
       <c r="I32" s="6">
@@ -1845,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7ECE8D-5EDB-484C-A8D0-768ED5127998}">
-  <dimension ref="B2:K9"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1883,10 +1870,10 @@
       <c r="E3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="38" t="s">
         <v>64</v>
       </c>
       <c r="H3" s="3"/>
@@ -1898,19 +1885,19 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="5">
         <v>10</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="39">
         <v>0.8</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="41">
         <f>E4*F4</f>
         <v>8</v>
       </c>
@@ -1923,10 +1910,10 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="47"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="40"/>
       <c r="G5" s="31"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1937,19 +1924,19 @@
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="2">
         <v>10</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="40">
         <v>0.9</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="41">
         <f>E6*F6</f>
         <v>9</v>
       </c>
@@ -1959,23 +1946,17 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="50">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="43">
         <f>SUM(G4:G6)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="41"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>